<commit_message>
Update Descriptive Stats - Teams.xlsx
</commit_message>
<xml_diff>
--- a/Analyses/Descriptive Stats - Teams.xlsx
+++ b/Analyses/Descriptive Stats - Teams.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/Omar/Documents/GitHub/team-eta/Analyses/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{1047D52C-14AA-A74F-8583-DCF9C975E7C7}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{C84F197E-86A0-1A47-945E-4C65382A5FCB}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="60" yWindow="460" windowWidth="25440" windowHeight="14640" xr2:uid="{B8937E31-6CED-CA47-B59F-63F9760627DC}"/>
   </bookViews>
@@ -815,9 +815,9 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{6364E291-8C9C-E540-B3F5-639C332BE116}">
   <dimension ref="A1:AZ721"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="AF1" zoomScale="90" zoomScaleNormal="90" workbookViewId="0">
+    <sheetView tabSelected="1" topLeftCell="AA1" zoomScale="90" zoomScaleNormal="90" workbookViewId="0">
       <pane ySplit="1" topLeftCell="A2" activePane="bottomLeft" state="frozen"/>
-      <selection pane="bottomLeft" activeCell="AT18" sqref="AT18"/>
+      <selection pane="bottomLeft" activeCell="AD8" sqref="AD8"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="16" x14ac:dyDescent="0.2"/>
@@ -969,7 +969,7 @@
         <v>64</v>
       </c>
       <c r="AG2" s="24" t="s">
-        <v>64</v>
+        <v>74</v>
       </c>
       <c r="AJ2" s="24" t="s">
         <v>64</v>

</xml_diff>